<commit_message>
shiftcal mutants filtering init
</commit_message>
<xml_diff>
--- a/mutant/mutation.xlsx
+++ b/mutant/mutation.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DroidShows" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ShiftCal" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ShiftCal - BWD - TWD" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="232">
   <si>
     <t xml:space="preserve">Mutant</t>
   </si>
@@ -1275,6 +1276,129 @@
 * Get more help at https://help.gradle.org
 BUILD FAILED in 4s
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_shift_creator.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button widget deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.google.android.material.floatingactionbutton.FloatingActionButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_shift_creator.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EditText widget deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EditText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">android.widget.Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_calendar.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImageButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_employer_creator.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_calendar.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_about.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_alarm.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_executed_alarm.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_shifts.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_employer_creator.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_theme.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_employers.xml</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1391,6 +1515,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3402,8 +3534,8 @@
   </sheetPr>
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4373,4 +4505,358 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="24.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="24.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
droidshows new mutation operators results
</commit_message>
<xml_diff>
--- a/mutant/mutation.xlsx
+++ b/mutant/mutation.xlsx
@@ -10,8 +10,10 @@
   <sheets>
     <sheet name="DroidShows" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ShiftCal" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ShiftCal-Result-B&amp;T" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="ShiftCal - BWD - TWD" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="DroidShows-Result-B&amp;T" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="DroidShows - BWD - TWD" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ShiftCal-Result-B&amp;T" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ShiftCal - BWD - TWD" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="242">
   <si>
     <t xml:space="preserve">Mutant</t>
   </si>
@@ -1285,10 +1287,64 @@
     <t xml:space="preserve">Button widget deletion</t>
   </si>
   <si>
+    <t xml:space="preserve">mutant_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EditText widget deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ddms]: Exception during activity from Selector.
+[ddms]: null
+java.nio.channels.CancelledKeyException
+	at java.base/sun.nio.ch.SelectionKeyImpl.ensureValid(SelectionKeyImpl.java:71)
+	at java.base/sun.nio.ch.SelectionKeyImpl.readyOps(SelectionKeyImpl.java:130)
+	at java.base/java.nio.channels.SelectionKey.isAcceptable(SelectionKey.java:425)
+	at com.android.ddmlib.internal.jdwp.JdwpProxyServer.runAsServer(JdwpProxyServer.java:281)
+	at com.android.ddmlib.internal.jdwp.JdwpProxyServer.run(JdwpProxyServer.java:321)
+	at java.base/java.lang.Thread.run(Thread.java:829)
+[ddms]: Exception during activity from Selector.
+[ddms]: null
+java.nio.channels.CancelledKeyException
+	at java.base/sun.nio.ch.SelectionKeyImpl.ensureValid(SelectionKeyImpl.java:71)
+	at java.base/sun.nio.ch.SelectionKeyImpl.readyOps(SelectionKeyImpl.java:130)
+	at java.base/java.nio.channels.SelectionKey.isAcceptable(SelectionKey.java:425)
+	at com.android.ddmlib.internal.jdwp.JdwpProxyServer.runAsServer(JdwpProxyServer.java:281)
+	at com.android.ddmlib.internal.jdwp.JdwpProxyServer.run(JdwpProxyServer.java:321)
+	at java.base/java.lang.Thread.run(Thread.java:829)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImageButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
     <t xml:space="preserve">mutant_2</t>
   </si>
   <si>
-    <t xml:space="preserve">EditText widget deletion</t>
+    <t xml:space="preserve">alert_about.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">mutant_3</t>
@@ -1300,13 +1356,28 @@
     <t xml:space="preserve">mutant_5</t>
   </si>
   <si>
-    <t xml:space="preserve">mutant_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mutant_8</t>
+    <t xml:space="preserve">add_serie.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mutant_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alert_filter.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ToggleButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EditText</t>
   </si>
   <si>
     <t xml:space="preserve">mutant_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row_serie_seasons.xml</t>
   </si>
   <si>
     <t xml:space="preserve">Warning: Mapping new ns http://schemas.android.com/repository/android/common/02 to old ns http://schemas.android.com/repository/android/common/01
@@ -1355,45 +1426,21 @@
     <t xml:space="preserve">mutant_18</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid</t>
-  </si>
-  <si>
     <t xml:space="preserve">activity_shift_creator.xml</t>
   </si>
   <si>
     <t xml:space="preserve">com.google.android.material.floatingactionbutton.FloatingActionButton</t>
   </si>
   <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
     <t xml:space="preserve">content_shift_creator.xml</t>
   </si>
   <si>
-    <t xml:space="preserve">EditText</t>
-  </si>
-  <si>
     <t xml:space="preserve">android.widget.Button</t>
   </si>
   <si>
-    <t xml:space="preserve">mutant_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
     <t xml:space="preserve">activity_calendar.xml</t>
   </si>
   <si>
-    <t xml:space="preserve">ImageButton</t>
-  </si>
-  <si>
     <t xml:space="preserve">activity_employer_creator.xml</t>
   </si>
   <si>
@@ -1404,9 +1451,6 @@
   </si>
   <si>
     <t xml:space="preserve">content_about.xml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button</t>
   </si>
   <si>
     <t xml:space="preserve">mutant_12</t>
@@ -1572,23 +1616,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -4567,9 +4594,286 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -4610,7 +4914,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>194</v>
@@ -4624,7 +4928,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>194</v>
@@ -4638,7 +4942,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>192</v>
@@ -4652,7 +4956,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>192</v>
@@ -4666,7 +4970,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>192</v>
@@ -4680,7 +4984,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>192</v>
@@ -4694,7 +4998,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>192</v>
@@ -4703,12 +5007,12 @@
         <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>192</v>
@@ -4717,12 +5021,12 @@
         <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>192</v>
@@ -4736,7 +5040,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>194</v>
@@ -4750,7 +5054,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>192</v>
@@ -4773,7 +5077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4798,16 +5102,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4815,305 +5119,305 @@
         <v>191</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>194</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>194</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>194</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>